<commit_message>
Final dashboard update with some minor changes and a new database
</commit_message>
<xml_diff>
--- a/proxy_data.xlsx
+++ b/proxy_data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="31">
   <si>
     <t>Student Name</t>
   </si>
@@ -22,64 +22,88 @@
     <t>Study Time</t>
   </si>
   <si>
+    <t>Havel</t>
+  </si>
+  <si>
+    <t>CS 391</t>
+  </si>
+  <si>
+    <t>MRKT 237</t>
+  </si>
+  <si>
+    <t>MTH 254</t>
+  </si>
+  <si>
+    <t>PH 212</t>
+  </si>
+  <si>
+    <t>Josh</t>
+  </si>
+  <si>
+    <t>WR 121</t>
+  </si>
+  <si>
+    <t>BA 348</t>
+  </si>
+  <si>
+    <t>CS 340</t>
+  </si>
+  <si>
+    <t>BANA 270</t>
+  </si>
+  <si>
+    <t>Kai</t>
+  </si>
+  <si>
+    <t>CS 162</t>
+  </si>
+  <si>
+    <t>MTH 251</t>
+  </si>
+  <si>
+    <t>CS 271</t>
+  </si>
+  <si>
+    <t>Omori</t>
+  </si>
+  <si>
+    <t>AI 537</t>
+  </si>
+  <si>
+    <t>AI 541</t>
+  </si>
+  <si>
+    <t>Owen</t>
+  </si>
+  <si>
+    <t>BIO 101</t>
+  </si>
+  <si>
+    <t>MTH 361</t>
+  </si>
+  <si>
+    <t>Paul</t>
+  </si>
+  <si>
+    <t>BANA 372</t>
+  </si>
+  <si>
+    <t>MTH 241</t>
+  </si>
+  <si>
+    <t>BANA 472</t>
+  </si>
+  <si>
+    <t>Tri</t>
+  </si>
+  <si>
     <t>Vi</t>
   </si>
   <si>
-    <t>MTH 241</t>
-  </si>
-  <si>
-    <t>Kai</t>
-  </si>
-  <si>
-    <t>CS 162</t>
-  </si>
-  <si>
-    <t>Tri</t>
-  </si>
-  <si>
-    <t>CS 340</t>
-  </si>
-  <si>
-    <t>Omori</t>
-  </si>
-  <si>
-    <t>MTH 251</t>
-  </si>
-  <si>
-    <t>Paul</t>
-  </si>
-  <si>
-    <t>BANA 372</t>
-  </si>
-  <si>
-    <t>Havel</t>
-  </si>
-  <si>
-    <t>CS 391</t>
-  </si>
-  <si>
-    <t>Owen</t>
-  </si>
-  <si>
-    <t>BIO 101</t>
-  </si>
-  <si>
-    <t>BANA 472</t>
-  </si>
-  <si>
-    <t>Josh</t>
-  </si>
-  <si>
-    <t>MTH 254</t>
-  </si>
-  <si>
-    <t>PH 212</t>
-  </si>
-  <si>
-    <t>WR 121</t>
-  </si>
-  <si>
-    <t>BA 348</t>
+    <t>ENG 100</t>
+  </si>
+  <si>
+    <t>BANA 450</t>
   </si>
 </sst>
 </file>
@@ -358,37 +382,37 @@
         <v>4</v>
       </c>
       <c r="C2" s="2">
-        <v>0.10416666666666667</v>
+        <v>0.041666666666666664</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="C3" s="2">
-        <v>0.2222222222222222</v>
+        <v>0.041666666666666664</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C4" s="2">
-        <v>0.16666666666666666</v>
+        <v>0.10416666666666667</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C5" s="2">
         <v>0.13541666666666666</v>
@@ -396,99 +420,347 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C6" s="2">
-        <v>0.08333333333333333</v>
+        <v>0.041666666666666664</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C7" s="2">
-        <v>0.041666666666666664</v>
+        <v>0.10416666666666667</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C8" s="2">
-        <v>0.006944444444444444</v>
+        <v>0.13541666666666666</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C9" s="2">
-        <v>0.2222222222222222</v>
+        <v>0.041666666666666664</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="C10" s="2">
-        <v>0.041666666666666664</v>
+        <v>0.2222222222222222</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C11" s="2">
-        <v>0.10416666666666667</v>
+        <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C12" s="2">
-        <v>0.13541666666666666</v>
+        <v>0.2222222222222222</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C13" s="2">
-        <v>0.041666666666666664</v>
+        <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.13541666666666666</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0.08333333333333333</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0.13541666666666666</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0.08333333333333333</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.006944444444444444</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0.041666666666666664</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C20" s="2">
+        <v>0.20833333333333334</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0.006944444444444444</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0.041666666666666664</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0.20833333333333334</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="2">
+        <v>0.08333333333333333</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="2">
+        <v>0.041666666666666664</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="2">
+        <v>0.08333333333333333</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0.041666666666666664</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" s="2">
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29" s="2">
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" s="2">
+        <v>0.10416666666666667</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" s="2">
+        <v>0.2222222222222222</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" s="2">
         <v>0.00625</v>
       </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" s="2">
+        <v>0.08333333333333333</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C34" s="2">
+        <v>0.10416666666666667</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35" s="2">
+        <v>0.2222222222222222</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C36" s="2">
+        <v>0.00625</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="C37" s="2"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>